<commit_message>
Update to .Net 8.0
</commit_message>
<xml_diff>
--- a/Docs/notes.xlsx
+++ b/Docs/notes.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="53">
   <si>
     <t>Danh sách làm việc theo bảng sql</t>
   </si>
@@ -93,6 +93,9 @@
   </si>
   <si>
     <t>Xây dựng Domain.Entities để nhận giá trị trong lớp xử lý Infrastructure</t>
+  </si>
+  <si>
+    <t>update đồ án lên .Net 8.0</t>
   </si>
   <si>
     <t>ChucVu</t>
@@ -845,7 +848,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -854,9 +857,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1417,8 +1417,8 @@
   <sheetPr/>
   <dimension ref="C1:J34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15"/>
@@ -1458,10 +1458,10 @@
       <c r="F3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="G3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H3" s="5"/>
+      <c r="H3" s="4"/>
       <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1470,476 +1470,476 @@
       </c>
     </row>
     <row r="4" spans="3:10">
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="G4" s="8" t="s">
+      <c r="G4" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="5"/>
-      <c r="I4" s="9" t="s">
+      <c r="H4" s="4"/>
+      <c r="I4" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="3:10">
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="7" t="s">
+      <c r="D5" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7" t="s">
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="9"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="9" t="s">
+      <c r="G5" s="8"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="3:10">
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="7" t="s">
+      <c r="D6" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7" t="s">
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G6" s="9"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="9" t="s">
+      <c r="G6" s="8"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="J6" s="11"/>
+      <c r="J6" s="10" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="7" spans="3:10">
-      <c r="C7" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="7" t="s">
+      <c r="C7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="H7" s="5"/>
-      <c r="I7" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="J7" s="9"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="7"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" spans="3:10">
-      <c r="C8" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="s">
+      <c r="C8" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E8" s="7"/>
-      <c r="F8" s="7" t="s">
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G8" s="9"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8" s="9"/>
+      <c r="G8" s="8"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" spans="3:10">
-      <c r="C9" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="7" t="s">
+      <c r="C9" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D9" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E9" s="7"/>
-      <c r="F9" s="7" t="s">
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="9"/>
-      <c r="J9" s="9"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="8"/>
+      <c r="J9" s="8"/>
     </row>
     <row r="10" spans="3:10">
-      <c r="C10" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E10" s="7"/>
-      <c r="F10" s="7" t="s">
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="9"/>
-      <c r="J10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" spans="3:10">
-      <c r="C11" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="7" t="s">
+      <c r="C11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E11" s="7"/>
-      <c r="F11" s="7" t="s">
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G11" s="9"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="9"/>
-      <c r="J11" s="9"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="3:10">
-      <c r="C12" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="7" t="s">
+      <c r="C12" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="7"/>
-      <c r="F12" s="7" t="s">
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="5"/>
-      <c r="I12" s="9"/>
-      <c r="J12" s="9"/>
+      <c r="G12" s="8"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" spans="3:10">
-      <c r="C13" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="7" t="s">
+      <c r="C13" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D13" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E13" s="7"/>
-      <c r="F13" s="7" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="9"/>
-      <c r="J13" s="9"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" spans="3:10">
-      <c r="C14" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="7" t="s">
+      <c r="C14" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E14" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="7" t="s">
+      <c r="E14" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="5"/>
-      <c r="I14" s="9"/>
-      <c r="J14" s="9"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="8"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="3:10">
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D15" s="7" t="s">
+      <c r="F15" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="8"/>
+      <c r="J15" s="8"/>
+    </row>
+    <row r="16" spans="3:10">
+      <c r="C16" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F15" s="7" t="s">
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="9"/>
-      <c r="J15" s="9"/>
-    </row>
-    <row r="16" spans="3:10">
-      <c r="C16" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D16" s="7" t="s">
+      <c r="G16" s="8"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="8"/>
+      <c r="J16" s="8"/>
+    </row>
+    <row r="17" spans="3:10">
+      <c r="C17" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7" t="s">
+      <c r="E17" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="5"/>
-      <c r="I16" s="9"/>
-      <c r="J16" s="9"/>
-    </row>
-    <row r="17" spans="3:10">
-      <c r="C17" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D17" s="7" t="s">
+      <c r="G17" s="8"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+    </row>
+    <row r="18" spans="3:10">
+      <c r="C18" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="8"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+    </row>
+    <row r="19" spans="3:10">
+      <c r="C19" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D19" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E17" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F17" s="7" t="s">
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G17" s="9"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="9"/>
-    </row>
-    <row r="18" spans="3:10">
-      <c r="C18" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="9"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="9"/>
-      <c r="J18" s="9"/>
-    </row>
-    <row r="19" spans="3:10">
-      <c r="C19" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D19" s="7" t="s">
+      <c r="G19" s="8"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+    </row>
+    <row r="20" spans="3:10">
+      <c r="C20" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G20" s="8"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="3:10">
+      <c r="C21" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D21" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E19" s="7"/>
-      <c r="F19" s="7" t="s">
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G19" s="9"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="9"/>
-      <c r="J19" s="9"/>
-    </row>
-    <row r="20" spans="3:10">
-      <c r="C20" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7" t="s">
+      <c r="G21" s="8"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="3:10">
+      <c r="C22" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+    </row>
+    <row r="23" spans="3:10">
+      <c r="C23" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G20" s="9"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="9"/>
-      <c r="J20" s="9"/>
-    </row>
-    <row r="21" spans="3:10">
-      <c r="C21" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D21" s="7" t="s">
+      <c r="G23" s="8"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="3:10">
+      <c r="C24" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E21" s="7"/>
-      <c r="F21" s="7" t="s">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G21" s="9"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="9"/>
-      <c r="J21" s="9"/>
-    </row>
-    <row r="22" spans="3:10">
-      <c r="C22" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="9"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="9"/>
-    </row>
-    <row r="23" spans="3:10">
-      <c r="C23" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D23" s="7" t="s">
+      <c r="G24" s="8"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="3:10">
+      <c r="C25" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D25" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E23" s="7"/>
-      <c r="F23" s="7" t="s">
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G23" s="9"/>
-      <c r="H23" s="5"/>
-      <c r="I23" s="9"/>
-      <c r="J23" s="9"/>
-    </row>
-    <row r="24" spans="3:10">
-      <c r="C24" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D24" s="7" t="s">
+      <c r="G25" s="8"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="3:10">
+      <c r="C26" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E24" s="7"/>
-      <c r="F24" s="7" t="s">
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="G24" s="9"/>
-      <c r="H24" s="5"/>
-      <c r="I24" s="9"/>
-      <c r="J24" s="9"/>
-    </row>
-    <row r="25" spans="3:10">
-      <c r="C25" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G25" s="9"/>
-      <c r="H25" s="5"/>
-      <c r="I25" s="9"/>
-      <c r="J25" s="9"/>
-    </row>
-    <row r="26" spans="3:10">
-      <c r="C26" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G26" s="9"/>
-      <c r="H26" s="5"/>
-      <c r="I26" s="9"/>
-      <c r="J26" s="9"/>
+      <c r="G26" s="8"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
     </row>
     <row r="27" spans="3:10">
-      <c r="C27" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="5"/>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
+      <c r="C27" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D27" s="6"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
     </row>
     <row r="28" spans="3:10">
-      <c r="C28" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="5"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
+      <c r="C28" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="8"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
     </row>
     <row r="29" spans="3:10">
-      <c r="C29" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
+      <c r="C29" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
     </row>
     <row r="30" spans="3:10">
-      <c r="C30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="5"/>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
+      <c r="C30" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="8"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
     </row>
     <row r="31" spans="3:10">
-      <c r="C31" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="9"/>
+      <c r="C31" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="4"/>
+      <c r="I31" s="8"/>
+      <c r="J31" s="8"/>
     </row>
     <row r="32" spans="3:10">
-      <c r="C32" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="5"/>
-      <c r="I32" s="9"/>
-      <c r="J32" s="9"/>
+      <c r="C32" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="8"/>
+      <c r="H32" s="4"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
     </row>
     <row r="33" spans="3:10">
-      <c r="C33" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="7"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="9"/>
-      <c r="J33" s="9"/>
+      <c r="C33" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="4"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
     </row>
     <row r="34" spans="4:5">
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>